<commit_message>
project updated and added selenium grid code
</commit_message>
<xml_diff>
--- a/src/test/resources/UseCaseData/ParaBank_TestCases.xlsx
+++ b/src/test/resources/UseCaseData/ParaBank_TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Believe_IT_Project\POC\ParaBank_SeleniumFramework\src\test\resources\UseCaseData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B765AC4-3A7E-48A0-A7C6-B9D29CDD9E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C982EA-FC6F-4E34-9647-0449947F4527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Scenarios" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="135">
   <si>
     <t>Project Name</t>
   </si>
@@ -133,9 +133,6 @@
     <t xml:space="preserve">Test Scenario </t>
   </si>
   <si>
-    <t xml:space="preserve">Test Case Description </t>
-  </si>
-  <si>
     <t>TC_RF_001</t>
   </si>
   <si>
@@ -163,9 +160,6 @@
     <t>987-65-4321</t>
   </si>
   <si>
-    <t>Verify that user is able to login successfully in the ParaBank application after providing the valid username and password</t>
-  </si>
-  <si>
     <t>TC_LF_001</t>
   </si>
   <si>
@@ -376,16 +370,82 @@
     <t>TC_TF_002</t>
   </si>
   <si>
+    <t>Verify that the user able to update address and phone number field from Update profile page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your updated address and phone number have been added to the system. </t>
+  </si>
+  <si>
+    <t>TestCaseDescription</t>
+  </si>
+  <si>
+    <t>FeatureName</t>
+  </si>
+  <si>
+    <t>TesterName</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>SignUp</t>
+  </si>
+  <si>
+    <t>OpenNewAccount</t>
+  </si>
+  <si>
+    <t>AccountOverview</t>
+  </si>
+  <si>
+    <t>TransferFunds</t>
+  </si>
+  <si>
+    <t>BillPay</t>
+  </si>
+  <si>
+    <t>Pranjali</t>
+  </si>
+  <si>
+    <t>Sagar</t>
+  </si>
+  <si>
+    <t>TC_LF_002</t>
+  </si>
+  <si>
+    <t>wrong@123</t>
+  </si>
+  <si>
+    <t>Verify that user is able to login successfully in the ParaBank application with valid username and password</t>
+  </si>
+  <si>
+    <t>Verify that user is able to login successfully in the ParaBank application with invalid username and password</t>
+  </si>
+  <si>
+    <t>UpdateContactInfo</t>
+  </si>
+  <si>
+    <t>mike@1234</t>
+  </si>
+  <si>
     <t>harry</t>
   </si>
   <si>
-    <t>harry@123</t>
-  </si>
-  <si>
-    <t>Verify that the user able to update address and phone number field from Update profile page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your updated address and phone number have been added to the system. </t>
+    <t>michael</t>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>MicrosoftEdge</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>firefox</t>
+  </si>
+  <si>
+    <t>mike</t>
   </si>
 </sst>
 </file>
@@ -503,7 +563,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -568,6 +628,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -996,10 +1062,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{168922AD-A63C-493F-9B16-63CA16C25E27}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1007,187 +1073,265 @@
     <col min="1" max="1" width="12.33203125" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.109375" style="10" customWidth="1"/>
     <col min="3" max="3" width="62.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="52.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.109375" style="9" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="52.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>29</v>
       </c>
       <c r="C1" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="N1" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="O1" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="P1" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q1" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="R1" s="17" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="14" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
         <v>30</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="I1" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="K1" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="L1" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="M1" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="N1" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="O1" s="17" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" s="14" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
-        <v>31</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="G2" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="H2" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="I2" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="J2" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="K2" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="L2" s="12">
+        <v>90001</v>
+      </c>
+      <c r="M2" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="12">
-        <v>90001</v>
-      </c>
-      <c r="J2" s="12" t="s">
+      <c r="N2" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="K2" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="M2" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="N2" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>43</v>
+      <c r="O2" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="P2" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q2" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="R2" s="12" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{E247EF81-3AAF-44BC-A63E-8BB87D6CAC54}">
+      <formula1>"MicrosoftEdge,chrome,firefox"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BD22433-6D1E-44A0-A1E1-3F1ED0AD5C2C}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.21875" style="10" customWidth="1"/>
-    <col min="3" max="3" width="80.77734375" style="9" customWidth="1"/>
-    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.21875" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="79.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.109375" style="24" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.77734375" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>29</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>45</v>
+        <v>111</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>130</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="F2" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="12" t="s">
-        <v>34</v>
-      </c>
+    </row>
+    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F3" xr:uid="{F99EED38-9B01-4B2E-ACD2-94C26EAA1BED}">
+      <formula1>"MicrosoftEdge,chrome,firefox"</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{688B2F4F-A723-404A-8C5C-BB3560880665}"/>
+    <hyperlink ref="H3" r:id="rId1" xr:uid="{C1F53C83-D12C-4E41-A7D0-1457E40261CF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1195,10 +1339,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF86A546-9405-4D3F-9C75-26EF322A018B}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1206,128 +1350,179 @@
     <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.33203125" customWidth="1"/>
     <col min="3" max="3" width="71.21875" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" style="9" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="9" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" style="24" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>29</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>30</v>
+        <v>111</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>53</v>
+        <v>112</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I1" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="G2" s="13"/>
-    </row>
-    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" s="13"/>
+    </row>
+    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="E3" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" s="8"/>
-    </row>
-    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="8"/>
+    </row>
+    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="F5" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="H5" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" s="13" t="s">
         <v>48</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F5" xr:uid="{F5E68871-6C79-4F7C-BF94-0F791432EBA6}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I5" xr:uid="{F5E68871-6C79-4F7C-BF94-0F791432EBA6}">
       <formula1>"CHECKING, SAVINGS"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F5" xr:uid="{3458A1F0-C550-4A28-B97B-862237FB3E2F}">
+      <formula1>"MicrosoftEdge,chrome,firefox"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1336,10 +1531,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60B9F128-8CCB-41D4-94ED-A8FE0F0E1719}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E3"/>
+      <selection activeCell="E10" activeCellId="1" sqref="E4 E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1347,72 +1542,107 @@
     <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.33203125" customWidth="1"/>
     <col min="3" max="3" width="71.21875" style="21" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="9" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" style="24" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>29</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>30</v>
+        <v>111</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>53</v>
+        <v>112</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="E3" s="22" t="s">
-        <v>112</v>
+        <v>106</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F3" xr:uid="{FEBE463A-8B83-40E2-A925-1BEF3B9EC4C3}">
+      <formula1>"MicrosoftEdge,chrome,firefox"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65E08CE0-D04C-4390-AA78-67085784C0E3}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E3"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1420,88 +1650,123 @@
     <col min="1" max="1" width="11.21875" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.21875" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="67.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="9" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" style="24" customWidth="1"/>
+    <col min="7" max="7" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>29</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>30</v>
+        <v>111</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>53</v>
+        <v>112</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="14" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="14" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-    </row>
-    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+    </row>
+    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="E3" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="F3" s="12">
+        <v>69</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="I3" s="12">
         <v>2000</v>
       </c>
-      <c r="G3" s="12" t="s">
-        <v>74</v>
+      <c r="J3" s="12" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F3" xr:uid="{83F954FB-678E-4C2D-8B8A-1F5B0FDBEC4F}">
+      <formula1>"MicrosoftEdge,chrome,firefox"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE7A1FD8-068A-4407-9B8B-5684EDD485E3}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1509,114 +1774,140 @@
     <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="9" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" style="24" customWidth="1"/>
+    <col min="7" max="7" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>29</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>30</v>
+        <v>111</v>
       </c>
       <c r="D1" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="L1" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="M1" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="O1" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="P1" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="I1" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="J1" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="K1" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="L1" s="17" t="s">
+      <c r="Q1" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="M1" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="N1" s="17" t="s">
+      <c r="R1" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="O1" s="17" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" s="14" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:18" s="14" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="F2" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="M2" s="12">
+        <v>10001</v>
+      </c>
+      <c r="N2" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="G2" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="J2" s="12">
-        <v>10001</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="L2" s="12">
+      <c r="O2" s="12">
         <v>14554</v>
       </c>
-      <c r="M2" s="12">
+      <c r="P2" s="12">
         <v>14554</v>
       </c>
-      <c r="N2" s="12">
+      <c r="Q2" s="12">
         <v>200</v>
       </c>
-      <c r="O2" s="12" t="s">
-        <v>81</v>
+      <c r="R2" s="12" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{53102AD8-2400-46A9-A27C-892048AC554A}">
+      <formula1>"MicrosoftEdge,chrome,firefox"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1644,121 +1935,121 @@
   <sheetData>
     <row r="1" spans="1:8" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>29</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>30</v>
+        <v>111</v>
       </c>
       <c r="D1" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="G1" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="H1" s="17" t="s">
         <v>91</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="14" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>24</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>24</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
       <c r="H4" s="15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H5" s="15"/>
     </row>
@@ -1770,10 +2061,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14C2D041-F53E-4671-8961-3FF77C44FF94}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1781,87 +2072,113 @@
     <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="57.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="61.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" style="9" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="9" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" style="24" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="61.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="11" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="11" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>29</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>30</v>
+        <v>111</v>
       </c>
       <c r="D1" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="K1" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="17" t="s">
+      <c r="L1" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="I1" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="K1" s="17" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="14" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="N1" s="17" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="14" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>25</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="F2" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="K2" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="L2" s="12">
+        <v>33101</v>
+      </c>
+      <c r="M2" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="H2" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="I2" s="12">
-        <v>33101</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>114</v>
+      <c r="N2" s="12" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{A947FB39-568E-404B-83CE-D44393E27C0B}">
+      <formula1>"MicrosoftEdge,chrome,firefox"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>